<commit_message>
[ENH] budget plan, finish unit based template
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_plan_unit_base.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_plan_unit_base.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Expense" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Revenue" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Activity Group" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="JorOder" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Job Order" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="ChargeType" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t xml:space="preserve">Financial Year</t>
   </si>
@@ -139,242 +139,6 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">การจัดหาครุภัณฑ์ เครื่องมือ อุปกรณ์ และระบบงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การซื้อครุภัณฑ์  เครื่องมือ อุปกรณ์ และระบบงานคอมพิวเตอร์   License Software </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าตอบแทนและการจ้างปฏิบัติงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าจ้างที่มาทำงานให้ สวทช. เช่น จ่ายค่าตอบแทน ค่าที่ปรึกษา นักศึกษาฝึกงาน จ้าง helpdesk  โปรแกรมเมอร์ ค่าสอบบัญชี  ค่าตรวจประเมิน ISO รวมถึงการค่าจ้างบริหารจัดการ Organizer ค่าทำความสะอาด ค่าซักรีด ค่าล้างหลอดทดลอง (นอกเหนือจากสัญญาใหญ่เป็นรายครั้ง)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าเช่าอุปกรณ์ สถานที่และใช้บริการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าเช่าทุกประเภท รวมถึงค่าเช่าถ่ายเอกสารพร้อมค่าจ้างคนถ่ายเอกสาร    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การบริหารจัดการและบำรุงรักษาระบบงานต่าง ๆ  (ระบบอาคารสถานที่ ครุภัณฑ์ และอุปกรณ์ต่างๆ )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายในการบริหารจัดการและบำรุงรักษาต่างๆ ครุภัณฑ์ เครื่องมือ อุปกรณ์  ระบบงาน  และ ต่ออายุ  License   ต่ออายุ Domain  ระบบเครือข่ายช่องสัญญาณ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การซ่อมแซม  อาคาร สถานที่  ระบบประกอบอาคาร รวมทั้ง ครุภัณฑ์  เครื่องมือ และอุปกรณ์ต่างๆ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายที่ใช้ในการซ่อมแซมอาคาร สถานที่ ระบบประกอบอาคาร ครุภัณฑ์ เครื่องมือ   และอุปกรณ์ต่างๆ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดประชุม</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดประชุมหารือปฏิบัติงาน และบริหารงาน ทั้งภายในและภายนอกสวทช. รวมถึง ค่าประชุมบอร์ดต่างๆ _x000D_
-_x000D_
-หมายเหตุ ขอลบคำว่า หารือปฏิบัติงาน และบริหารงาน เนื่องจากสับสนกับการปฏิบัติงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดกิจกรรม เผยแพร่ และ ผลิตสื่อ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การไปจัดนิทรรศการ เผยแพร่ การจัดทำสื่อต่างๆ เพื่อ นำผลงานไปสู่หน่วยงานภายนอก </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดฝึกอบรม สัมมนา พัฒนาบุคลากร สวทช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดฝึกอบรม สัมมนา พัฒนาบุคลากร สวทช.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดฝึกอบรม สัมมนา บุคลากรภายนอก</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดฝึกอบรม สัมมนา บุคลากรภายนอก ทั้งภายในประเทศ และ ต่างประเทศ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การสร้างภาพลักษณ์องค์กร</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดงานแถลงข่าว การจัดงานรับรอง การลงนาม MOU  และต้อนรับอย่างเป็นทางการที่สร้างภาพลักษณ์ขององค์กร</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเข้ารับการพัฒนาบุคลากร-ในประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การไปอบรมที่หน่วยงานภายนอกจัดอบรมภาย-ในประเทศ   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเข้ารับการพัฒนาบุคลากร-ต่างประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การไปอบรมที่หน่วยงานภายนอกจัดอบรมในต่างประเทศ (รวมหมายถึง การอบรมครั้งนั้น วัตถุประสงค์หลักคือไปอบรม-ต่างประเทศ แต่มีหลักสูตรที่มีการอบรมภายในประเทศด้วย) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางเสนอผลงาน-ในประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางเสนอผลงานภายในประเทศ  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางเสนอผลงาน-ต่างประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางเสนอผลงาน-ต่างประเทศ  (รวมหมายถึง  การเสนอผลงานครั้งนั้นมีวัตถุประสงค์หลักคือไปเสนอผลงานต่างประเทศ แต่มีต้องนำเสนอผลงานภายในประเทศด้วย) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางปฏิบัติงาน-ในประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางปฏิบัติงานภายในประเทศ เช่น เดินทางไปเข้าร่วมประชุม เดินทางไปซื้อของ เป็นต้น  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางปฏิบัติงาน-ต่างประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การเดินทางปฏิบัติงานต่างประเทศ (รวมทั้งคชจ. อื่นครั้งนั้นมีวัตถุประสงค์หลักคือการเดินทางไปปฏิบัติงานต่างประเทศ แต่มีต้องเดินทางภายในประเทศด้วย ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าวัสดุ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">วัสดุทุกประเภทที่จัดซื้อตามวัตถุประสงค์เนื้องานของกิจกรรม    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าวัสดุและครุภัณฑ์เพื่อใช้ทำต้นแบบ/ส่งมอบ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">วัสดุ และ ครุภัณฑ์เพื่อส่งมอบ และ ครุภัณฑ์วิจัยภายใน เช่น ซื้อมอเตอร์ไซด์ เพื่อเป็นต้นแบบวิจัย </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การประเมินหน่วยงานและโครงการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การประเมินผลงานของหน่วยงานและโครงการทั้งประเทศและต่างประเทศ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าวิเคราะห์และทดสอบ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายที่ใช้ในการวิเคราะห์และทดสอบ    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดทำรายงานและเอกสาร </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายที่เกี่ยวข้องกับการใช้ในการจัดทำรายงานและเอกสาร เช่น ค่ากระดาษ ค่ากระดาษกาว ค่าพิมพ์สี ค่าถ่ายเอกสารเพื่อจัดทำรายงาน ฯลฯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าวารสาร สมาชิก ใช้สิทธิ์และข้อมูล</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าสมัครสมาชิกวารสาร  ค่าใช้จ่ายในการซื้อลิขสิทธิ์ และฐานข้อมูล ทั้งในประเทศและต่างประเทศ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าโทรศัพท์ ค่า Internet  และค่าสาธารณูปโภค</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าไฟฟ้า และคำน้ำประปา ค่าโทรศัพท์และโทรคมนาคม _x000D_
--ค่าโทรศัพท์และโทรคมนาคม_x000D_
--ค่าไฟฟ้าและค่าน้ำประปา_x000D_
--ค่าขนส่งพัสดุ รับส่งเอกสาร และค่าไปรษณีย์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายเบ็ดเตล็ด</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายอื่นๆ  เช่น ค่าโทรศัพท์ ค่าไปรษณีย์ ค่าขนส่ง</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดการความปลอดภัย ชีวอนามัยและสิ่งแวดล้อม</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การจัดการความปลอดภัยที่มีผลกระทบต่อสิ่งแวดล้อม เช่น    บ่อบัดน้ำ การตรวจร่างการใน Lab ที่มีความเสี่ยง  ค่าวิเคราะห์อากาศ แสงเสียง ค่าซักเสื้อกาวน์ ฯลฯ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">การก่อสร้างและปรับปรุงอาคาร สถานที่และระบบอาคาร</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การสร้างอาคาร ขยายอาคาร และพื้นที่  รวมถึงการวางระบบใหม่ๆ ภายในอาคาร เช่น  วางระบบแอร์ ฯลฯ เพื่อเพิ่มประสิทธิภาพขยายอายุการใช้งาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินสนับสนุนและอุดหนุน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินสนับสนุนและอุดหนุนต่างๆ ให้หน่วยงานหรือบุคคลภายนอก</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินเดือนและสวัสดิการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินเดือนและสวัสดิการของพนักงาน/โครงการ สวทช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินตอบแทนอื่นสำหรับพนักงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าสมนาคุณพิเศษ (ส่วนแบ่งจากการทำงาน) รวมถึง ค่าวิทยาการ  ค่าตอบแทน Royalty  fee, ค่าตอบแทนสิทธิบัตร-พนักงาน, ค่าตอบแทนสิทธิบัตร-บุคคลภายนอก(มีระเบียบรองรับ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าสันทนาการและค่าใช้จ่ายเบ็ตเตล็ดของพนักงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ค่าใช้จ่ายที่เกี่ยวกับขวัญ-กำลังใจ และสันทนาการต่างๆ ของพนักงาน เช่น ค่ากระเช้าดอกไม้ ของที่ระลึก พวงหรีด งานกีฬาสี เงินช่วยเหลือค่าทำศพ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้จากงบประมาณแผ่นดิน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินได้ที่มาจากงบประมาณแผ่นดิน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เงินอุดหนุนรับ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้ที่รับการอุดหนุนต่างๆ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้จากการรับจ้างวิจัย/ร่วมวิจัย</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้ลิขสิทธิ์/สิทธิประโยชน์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้บริการเทคนิค/วิชาการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้ค่าที่ปรึกษาและวิเคราะห์ระบบงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้ค่าเช่าและบริการสถานที่</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้จัดฝึกอบรม/สัมนา/นิทรรศการ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้จากขายหนังสือ วารสาร สื่อมัลติมีเดีย และของที่ระลึก</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้อื่นจากการดำเนินงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้อื่นๆ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้ระหว่างภายใน สวทช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ดอกเบี้ยรับและเงินปันผล</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายได้อื่นๆ นอกเหนือจากดำเนินงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายการพิเศษ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Job Order Type</t>
   </si>
   <si>
@@ -382,399 +146,6 @@
   </si>
   <si>
     <t xml:space="preserve">Job Order Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Short text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">หน่วยงาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ศูนย์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nanosymposium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">กลาง</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global Young Scientists Summit (GYSS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GYSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การประชุมวิชาการประจำปี สวทช. (NAC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การประชุมวิชาการนานาชาติ (IAC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">งานประชุมวิชาการและนิทรรศการระดับนานาชาติทางนาโนเทคโนโลยี (นาโนไทยแลนด์)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NANOThailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">มหกรรมวิทยาศาสตร์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สัปดาห์วิทย์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International Conference on Polymer Characterization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การประชุมผู้บริหาร คอบช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">คอบช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asia-Pacific Advanced Network (APAN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Southeast Asia International Joint Research and Training Program(SEAIP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEAIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ประชุมวิชาการนานาชาติและงานแสดงนิทรรศการนานาชาติ (BIOAsia)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BioAsia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">กิจกรรมดูงานนอกสถานที่ Site Visit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Visit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIG Cleaning Day และ 5 ส</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 ส</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSTDA DAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HROD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">งานกีฬาสี สวทช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">กีฬาสี  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">กิจกรรมกีฬาเชื่อมความสัมพันธ์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">กีฬาเชื่อม</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NECTEC Annual Conference and Exhibition (NECTEC ACE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NECTEC ACE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ศอ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">การประชุม CASP2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ศว.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161019</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BIOTEC RADP CONFERENCE 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ศช.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODE MANIA100:CODING DEFINES ANYTHING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J161021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NANOTALK </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ศน.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">จัดฝึกอบรม</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMUNICATION DAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM DAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สก</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Competency development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional Development </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R&amp;D Generic Development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R&amp;D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDP &amp; HRD Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT IDP  (ICT Policy Development) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICT Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle Management Refreshment Program (MMRP) (Prepare/Perform/Progress)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MMRP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fundamental Management Program (FMP) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English Development (Academic/Business/Consulting)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English Academic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSTDA IT  development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSTDA IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety &amp; Quality &amp; Environement Development &amp; Risk Mgnt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Staff Orientation (R&amp;D and Non-R&amp;D)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knowledge Sharing (Generic + Occatioal + Hot issues)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mentoring program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mentoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620015</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> โปรแกรมจัดกิจกรรมพัฒนาศักยภาพบุคลากร ภายใต้ ที่ประชุมผู้บริหารหนว่ยงานพรบ.เฉพาะ (ทอพ.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ทอพ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">นักเรียนทุนที่สำเร็จการศึกษา</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">บริหารโครงการสนับสนุนนักเรียนทุนรัฐบาลฯ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สัมมนาเตรียมความพร้อมทุนบุคคลทั่วไป</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สัมมนาเตรียมความพร้อมทุนพัฒนาบุคลากรภาครัฐ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สัมมนาเตรียมความพร้อมทุนมัธยมศึกษาตอนปลาย</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">อบรมหลักสูตร ISO / OHSAS 18001:2015 Lead Auditor (IRCA Certified)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">อบรมเฉพาะกลุ่มหลักสูตร ความรู้พื้นฐาน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1620023</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INTERNATIONAL CONFERENCE ON SUSTAINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ศจ.</t>
   </si>
   <si>
     <t xml:space="preserve">External</t>
@@ -794,12 +165,13 @@
     <numFmt numFmtId="167" formatCode="* #,##0\ ;\-* #,##0\ ;* &quot;- &quot;;@\ "/>
     <numFmt numFmtId="168" formatCode="0\ ;\-0\ ;0\ ;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -821,11 +193,13 @@
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -833,12 +207,14 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -846,17 +222,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1064,7 +436,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1237,23 +609,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1267,22 +627,11 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
         <name val="Calibri"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
@@ -1363,19 +712,19 @@
   </sheetPr>
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="24" min="11" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="257" min="25" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0404858299595"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="31.82995951417"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="1" width="12.9757085020243"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.3238866396761"/>
+    <col collapsed="false" hidden="false" max="24" min="11" style="1" width="12.9757085020243"/>
+    <col collapsed="false" hidden="false" max="257" min="25" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3844,12 +3193,12 @@
       <formula1>ChargeType!$A$1:$A$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B59" type="list">
-      <formula1>'Activity Group'!$A$2:$A$25</formula1>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10:C59" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10:C59" type="list">
-      <formula1>JorOder!$C$2:$C$45</formula1>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B59" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3870,19 +3219,19 @@
   </sheetPr>
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="24" min="11" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="257" min="25" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0404858299595"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="31.82995951417"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="1" width="12.9757085020243"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.3238866396761"/>
+    <col collapsed="false" hidden="false" max="24" min="11" style="1" width="12.9757085020243"/>
+    <col collapsed="false" hidden="false" max="257" min="25" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6352,11 +5701,11 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10:C59" type="list">
-      <formula1>JorOder!$C$2:$C$45</formula1>
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10:B59" type="list">
-      <formula1>'Activity Group'!$A$35:$A$43</formula1>
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -6375,18 +5724,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="77.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="244.874493927125"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="39" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="78.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="251.085020242915"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="39" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" s="42" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6397,356 +5746,239 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46"/>
-      <c r="B32" s="46"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="B36" s="44" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
+    <row r="1048345" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048346" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048347" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048348" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048349" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048350" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048351" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048352" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048353" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048354" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048355" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048356" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048357" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048358" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048359" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048360" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048361" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048362" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048363" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048364" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048365" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048366" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048367" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048368" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048369" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048370" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048371" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048372" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048373" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048374" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048375" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048376" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048377" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048378" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048379" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048380" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048381" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048382" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048383" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048384" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048385" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048386" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048387" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048388" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048389" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048390" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048391" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048392" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048393" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048394" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048395" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048396" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048397" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048398" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048399" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048400" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048401" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048402" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048403" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048404" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048405" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048406" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048407" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048408" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048409" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048410" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048411" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048412" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048413" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048414" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048415" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048416" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048417" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048418" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048419" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048420" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048421" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048422" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048423" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048424" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048425" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048426" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048427" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048428" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048429" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048430" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048431" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048432" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048433" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048434" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048435" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048436" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048437" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048438" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048439" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048440" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048441" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048442" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048443" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048444" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048445" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048446" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048448" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048449" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048450" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048451" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048452" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048453" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048454" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048455" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048456" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048457" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6762,882 +5994,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="39" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="79.8016194331984"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="39" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="39" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="12.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="12.6882591093117"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="28.8421052631579"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="13.6275303643725"/>
+    <col collapsed="false" hidden="false" max="255" min="5" style="39" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="0"/>
-      <c r="E8" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>169</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19" s="0"/>
-      <c r="E19" s="44" t="n">
-        <v>305004</v>
-      </c>
-      <c r="F19" s="44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" s="0"/>
-      <c r="E20" s="44" t="n">
-        <v>205017</v>
-      </c>
-      <c r="F20" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="0"/>
-      <c r="E21" s="44" t="n">
-        <v>305004</v>
-      </c>
-      <c r="F21" s="44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22" s="44" t="n">
-        <v>602005</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>185</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="C24" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>191</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>198</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>200</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>201</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>202</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>204</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>205</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="C30" s="44" t="s">
-        <v>207</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>208</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="C31" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="C32" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="C33" s="44" t="s">
-        <v>216</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="E33" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="C34" s="44" t="s">
-        <v>219</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="C35" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="D35" s="44" t="s">
-        <v>223</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="C36" s="44" t="s">
-        <v>225</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="E36" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F36" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="C37" s="44" t="s">
-        <v>228</v>
-      </c>
-      <c r="D37" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="E37" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F37" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="E38" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F38" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C39" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="E39" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>234</v>
-      </c>
-      <c r="C40" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="E40" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F40" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>236</v>
-      </c>
-      <c r="C41" s="44" t="s">
-        <v>237</v>
-      </c>
-      <c r="E41" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F41" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="C42" s="44" t="s">
-        <v>239</v>
-      </c>
-      <c r="E42" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="F42" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>240</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>241</v>
-      </c>
-      <c r="E43" s="0"/>
-      <c r="F43" s="44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="C44" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="E44" s="44" t="n">
-        <v>302004</v>
-      </c>
-      <c r="F44" s="44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>244</v>
-      </c>
-      <c r="C45" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="E45" s="44" t="n">
-        <v>203002</v>
-      </c>
-      <c r="F45" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="44" t="s">
-        <v>246</v>
-      </c>
-      <c r="E46" s="44" t="n">
-        <v>504003</v>
-      </c>
-      <c r="F46" s="44" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0"/>
-      <c r="B47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="44" t="s">
-        <v>246</v>
-      </c>
-      <c r="B48" s="44" t="s">
-        <v>246</v>
-      </c>
+    <row r="1" s="43" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AMI1" s="44"/>
+      <c r="AMJ1" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7655,23 +6044,23 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>248</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>249</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>